<commit_message>
Feat : Do compare experiment
</commit_message>
<xml_diff>
--- a/final_project/result_df.xlsx
+++ b/final_project/result_df.xlsx
@@ -503,7 +503,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0.2654916768096046</v>
+        <v>0.2654916768096037</v>
       </c>
     </row>
     <row r="4">
@@ -549,7 +549,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0.3512155592087045</v>
+        <v>0.3512155592087044</v>
       </c>
     </row>
     <row r="6">
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>0.0237058729592538</v>
+        <v>0.02370587295925319</v>
       </c>
     </row>
     <row r="7">
@@ -595,7 +595,7 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>0.4595754056209778</v>
+        <v>0.4595754056209773</v>
       </c>
     </row>
     <row r="8">
@@ -618,7 +618,7 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>0.7519365287600156</v>
+        <v>0.751936528760016</v>
       </c>
     </row>
     <row r="9">
@@ -641,7 +641,7 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>0.008798633135227732</v>
+        <v>0.008798633135227774</v>
       </c>
     </row>
     <row r="10">
@@ -664,7 +664,7 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>0.05807386234859365</v>
+        <v>0.05807386234859468</v>
       </c>
     </row>
     <row r="11">
@@ -1032,7 +1032,7 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>0.3467087914829524</v>
+        <v>0.3467087914829531</v>
       </c>
     </row>
     <row r="27">
@@ -1055,7 +1055,7 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>0.03356859301114045</v>
+        <v>0.03356859301114068</v>
       </c>
     </row>
     <row r="28">
@@ -1078,7 +1078,7 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>0.1168686835528817</v>
+        <v>0.1168686835528796</v>
       </c>
     </row>
     <row r="29">
@@ -1101,7 +1101,7 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>0.2366885770133637</v>
+        <v>0.2366885770133627</v>
       </c>
     </row>
     <row r="30">
@@ -1124,7 +1124,7 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>0.01845354186361954</v>
+        <v>0.01845354186362047</v>
       </c>
     </row>
     <row r="31">
@@ -1147,7 +1147,7 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>0.5196005558477781</v>
+        <v>0.519600555847777</v>
       </c>
     </row>
     <row r="32">
@@ -1193,7 +1193,7 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>0.9791057629167598</v>
+        <v>0.9791057629167601</v>
       </c>
     </row>
     <row r="34">
@@ -1216,7 +1216,7 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>0.0001005287297383703</v>
+        <v>0.0001005287297389801</v>
       </c>
     </row>
     <row r="35">
@@ -1239,7 +1239,7 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>0.04058689403404379</v>
+        <v>0.04058689403404514</v>
       </c>
     </row>
     <row r="36">
@@ -1262,7 +1262,7 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>0.8351615274703622</v>
+        <v>0.8351615274703628</v>
       </c>
     </row>
     <row r="37">
@@ -1308,7 +1308,7 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>0.2483042456897674</v>
+        <v>0.2483042456897669</v>
       </c>
     </row>
     <row r="39">
@@ -1331,7 +1331,7 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>0.4162894474505976</v>
+        <v>0.4162894474505975</v>
       </c>
     </row>
   </sheetData>

</xml_diff>